<commit_message>
- The reviewed version is complete.
</commit_message>
<xml_diff>
--- a/H07R80/Rleased/BOM/H07R8.xlsx
+++ b/H07R80/Rleased/BOM/H07R8.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H07R8x-Hardware\Rleased\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H07R8x-Hardware\H07R80\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813EE081-B4D0-4587-9B62-4FF4DB257F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7D5483-421E-4E75-83FB-ECE43C1E34AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2640" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H07R80" sheetId="1" r:id="rId1"/>
+    <sheet name="H07R8" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="155">
   <si>
     <t>Description</t>
   </si>
@@ -184,9 +184,6 @@
     <t>C5</t>
   </si>
   <si>
-    <t>C0603C104K8RACTU</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -214,18 +211,9 @@
     <t>https://octopart.com/rc0603fr-0710kl-yageo-40025538?r=sp</t>
   </si>
   <si>
-    <t>CAP CER 0.1 UF 10V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -244,16 +232,265 @@
     <t>R2</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10W Stereo Audio Amplifier (H07R80) </t>
-  </si>
-  <si>
-    <t>1/xx/2024</t>
-  </si>
-  <si>
-    <t>C1, C2, C4</t>
+    <t>https://octopart.com/cc0603krx7r9bb103-yageo-192938?r=sp</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB103</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c1608x5r1e474k080ac-tdk-25947645?r=sp</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>C1608X5R1E474K080AC</t>
+  </si>
+  <si>
+    <t>CAP CER 0.47UF 25V X5R 0603</t>
+  </si>
+  <si>
+    <t>C10, C11, C18, C19, C20, C22, C23, C24, C25, C27, C28, C39, C40</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100R</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R5, R10, R11, R12, R13, R14</t>
+  </si>
+  <si>
+    <t>RC0603FR-10100KL</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cl10b104ka8nnnc-samsung-19831573?r=sp</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>C8, C9, C13, C45</t>
+  </si>
+  <si>
+    <t>https://octopart.com/0603yc104k4t2a-avx+interconnect+%2F+elco-8120651</t>
+  </si>
+  <si>
+    <t>AVX CORPORATION</t>
+  </si>
+  <si>
+    <t>0603YC104K4T2A</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>C1, C2, C4, C6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cc0603kpx7r9bb101-yageo-25628258?r=sp</t>
+  </si>
+  <si>
+    <t>CC0603KPX7R9BB101</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C32, C38, C42, C43</t>
+  </si>
+  <si>
+    <t>R3, R6, R9</t>
+  </si>
+  <si>
+    <t>J1, J2, J3</t>
+  </si>
+  <si>
+    <t>TERM BLK 2POS SIDE ENT 3.5MM PCB</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>https://octopart.com/1751248-phoenix+contact-31334?r=sp</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>UMK107BJ105KA-T</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 50V X5R 0603</t>
+  </si>
+  <si>
+    <t>C12, C15, C16, C17, C33, C34, C35, C36, C37, C44</t>
+  </si>
+  <si>
+    <t>CL10A225KO8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 16V X5R 0603</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT4K70</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>A780EN476M1HLAS050</t>
+  </si>
+  <si>
+    <t>CAP ALUM HYB 47UF 20% 50V SMD</t>
+  </si>
+  <si>
+    <t>C30, C31</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ao3400a-alpha+%26+omega+semiconductor-10533924?r=spc#CadModels</t>
+  </si>
+  <si>
+    <t>Alpha &amp; Omega Semiconductor Inc.</t>
+  </si>
+  <si>
+    <t>AO3400A</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 30V 5.7A SOT23-3L</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>https://octopart.com/max9704etj%2B-analog+devices-40016343?r=sp</t>
+  </si>
+  <si>
+    <t>Analog Devices Inc./Maxim Integrated</t>
+  </si>
+  <si>
+    <t>MAX9704ETJ+</t>
+  </si>
+  <si>
+    <t>IC AMP CLASS D STEREO 16W 32TQFN</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>https://octopart.com/max9867etj%2Bt-analog+devices-124229035?r=sp</t>
+  </si>
+  <si>
+    <t>Maxim Integrated Products</t>
+  </si>
+  <si>
+    <t>MAX9867ETJ+T</t>
+  </si>
+  <si>
+    <t>IC STEREO AUD CODEC LP 32TQFN</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>https://octopart.com/mic5365-1.8yd5-tr-microchip-66803184?r=spc#CadModels</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MIC5365-1.8YD5-TR</t>
+  </si>
+  <si>
+    <t>IC REG LIN 1.8V 150MA TSOT23-5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ts3a44159rgtr-texas+instruments-5447085?r=spc#CadModels</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TS3A44159RGTR</t>
+  </si>
+  <si>
+    <t>IC SWITCH SPDTX4 450MOHM 16VQFN</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>CONN JACK STEREO 3.5MM SMD R/A</t>
+  </si>
+  <si>
+    <t>SJ-3524-SMT-TR</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>https://octopart.com/sj-3524-smt-tr-cui+devices-106234236?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rmcf0603ft100r-stackpole+electronics-19212927?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rmcf0603ft4k70-stackpole+electronics-19213269?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-10100kl-yageo-12819539?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/umk107bj105ka-t-taiyo+yuden-12090744?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cl10a225ko8nnnc-samsung-19018971?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/a780en476m1hlas050-kemet-133897287?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10W Stereo Audio Amplifier (H07R8) </t>
+  </si>
+  <si>
+    <t>R1, FB3, FB4, FB5, FB6</t>
   </si>
 </sst>
 </file>
@@ -1374,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G20"/>
+  <dimension ref="A2:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1438,8 +1675,8 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>74</v>
+      <c r="D5" s="18">
+        <v>45342</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="20"/>
@@ -1450,7 +1687,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1482,19 +1719,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
@@ -1502,7 +1739,7 @@
     </row>
     <row r="10" spans="1:7" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>22</v>
@@ -1520,101 +1757,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>55</v>
+        <v>100</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1751248</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F11" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F13" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="F14" s="16">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F15" s="16">
         <v>1</v>
@@ -1622,59 +1859,59 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="F16" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="F17" s="16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="F18" s="16">
         <v>1</v>
@@ -1682,41 +1919,381 @@
     </row>
     <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="F19" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C37" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D37" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E37" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F37" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1727,18 +2304,17 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E11" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E13" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E16" r:id="rId7" xr:uid="{CA2BC9B7-037F-4782-ACB8-2D8F29264691}"/>
-    <hyperlink ref="E18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E17" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E24" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E27" r:id="rId6" xr:uid="{CA2BC9B7-037F-4782-ACB8-2D8F29264691}"/>
+    <hyperlink ref="E31" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>